<commit_message>
fixed scada addresses for coils
added leading zeros to addresses less than 10k for proper load into kepware, also added code to properly handle Boolean records.
</commit_message>
<xml_diff>
--- a/python/xlsxfile/Chico.xlsx
+++ b/python/xlsxfile/Chico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynn/github/aatest/python/xlsxfile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B370953F-E5BF-5C40-B421-3A7662DB4E4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EE54F-B0CE-8046-903F-C62C61D68B46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="2280" windowWidth="28320" windowHeight="13740" xr2:uid="{4305449F-26ED-E04D-87C6-2AF85973C866}"/>
+    <workbookView xWindow="1780" yWindow="3620" windowWidth="37080" windowHeight="13740" xr2:uid="{4305449F-26ED-E04D-87C6-2AF85973C866}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>Units</t>
   </si>
@@ -135,6 +135,42 @@
   </si>
   <si>
     <t>Measurement_Type</t>
+  </si>
+  <si>
+    <t>Triplex Fault</t>
+  </si>
+  <si>
+    <t>Triplex_Fault</t>
+  </si>
+  <si>
+    <t>%M20</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Alarm</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Pump 1</t>
+  </si>
+  <si>
+    <t>South_Horizontal_Heat_Treat_Lvl_SW</t>
+  </si>
+  <si>
+    <t>South Horizontal Heater Lvl SW</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>South Heater Treater</t>
   </si>
 </sst>
 </file>
@@ -184,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -193,6 +229,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FB391E-D4E6-BE42-B833-DFC96ADD7865}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,11 +687,11 @@
         <v>24</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D6" si="0">RIGHT(C4, LEN(C4)-3)</f>
+        <f t="shared" ref="D4:D7" si="0">RIGHT(C4, LEN(C4)-3)</f>
         <v>256</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E6" si="1">D4+40001</f>
+        <f t="shared" ref="E4:E7" si="1">D4+40001</f>
         <v>40257</v>
       </c>
       <c r="F4" t="s">
@@ -739,6 +776,74 @@
       </c>
       <c r="L6" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <f>D7+10001</f>
+        <v>10021</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>1099</v>
+      </c>
+      <c r="E8">
+        <v>1099</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spreadsheet pull and validation working
able to pull from spreadsheet and validate and fill in needed fields as well as generate kepware load
</commit_message>
<xml_diff>
--- a/python/xlsxfile/Chico.xlsx
+++ b/python/xlsxfile/Chico.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lynn/github/aatest/python/xlsxfile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39EE54F-B0CE-8046-903F-C62C61D68B46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065B7AB3-3137-F847-ACE6-72B7D88AC10E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="3620" windowWidth="37080" windowHeight="13740" xr2:uid="{4305449F-26ED-E04D-87C6-2AF85973C866}"/>
+    <workbookView xWindow="21200" yWindow="2360" windowWidth="26820" windowHeight="14100" activeTab="1" xr2:uid="{4305449F-26ED-E04D-87C6-2AF85973C866}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Site" sheetId="2" r:id="rId1"/>
+    <sheet name="Tags" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="57">
   <si>
     <t>Units</t>
   </si>
@@ -155,9 +156,6 @@
     <t>Ok</t>
   </si>
   <si>
-    <t>Binary</t>
-  </si>
-  <si>
     <t>Pump 1</t>
   </si>
   <si>
@@ -171,13 +169,46 @@
   </si>
   <si>
     <t>South Heater Treater</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Site_Name</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Operator_id</t>
+  </si>
+  <si>
+    <t>IP_Address</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>HMS_Titanic</t>
+  </si>
+  <si>
+    <t>Winsor LLC</t>
+  </si>
+  <si>
+    <t>166.166.166.166</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,6 +223,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF4285F4"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -220,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -230,6 +268,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,12 +582,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B92566-6363-C549-8930-F0E7FE1D1106}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>502</v>
+      </c>
+      <c r="E2" s="5">
+        <v>39.235728999999999</v>
+      </c>
+      <c r="F2" s="5">
+        <v>104.683065</v>
+      </c>
+      <c r="G2">
+        <v>888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FB391E-D4E6-BE42-B833-DFC96ADD7865}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,11 +796,11 @@
         <v>24</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ref="D4:D7" si="0">RIGHT(C4, LEN(C4)-3)</f>
+        <f t="shared" ref="D4:D6" si="0">RIGHT(C4, LEN(C4)-3)</f>
         <v>256</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E7" si="1">D4+40001</f>
+        <f t="shared" ref="E4:E6" si="1">D4+40001</f>
         <v>40257</v>
       </c>
       <c r="F4" t="s">
@@ -805,21 +914,21 @@
         <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K7" t="s">
         <v>30</v>
       </c>
       <c r="L7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="C8">
         <v>1099</v>
@@ -837,13 +946,13 @@
         <v>40</v>
       </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" t="s">
         <v>45</v>
-      </c>
-      <c r="L8" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>